<commit_message>
Changes to the RISC-V Excel
</commit_message>
<xml_diff>
--- a/sims/RISC-V Instructions.xlsx
+++ b/sims/RISC-V Instructions.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Descriptions" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Instruction Set" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Single Cycle RV32I Control Logi" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Mnemonics" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="203">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -454,6 +455,237 @@
   </si>
   <si>
     <t xml:space="preserve">0001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mnemonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd, imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = imm &lt;&lt; 12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = pc + (imm &lt;&lt; 12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = pc + 4     |     pc = pc + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd, rs1, imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = pc + 4     |     pc = rs1 + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rs1, rs2, imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (rs1 == rs2)  pc = pc + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (rs1 != rs2)  pc = pc + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (rs1 &lt; rs2)  pc = pc + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed comparison and imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">if (rs1 &gt;= rs2)  pc = pc + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsigned comparison and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd, imm(rs1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = (m[rs1 + imm])[7:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loads 8 bits from memory and sign-extends it and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = (m[rs1 + imm])[15:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loads 16 bits from memory and sign-extends it and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = m[rs1 + imm]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loads 32 bits from memory and sign-extends it and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loads 8 bits from memory and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Loads 16 bits from memory and Signed imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rs2, imm(rs1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m[rs1 + imm] = rs2[7:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store 8-bits from lower bits of rs2 into memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m[rs1 + imm] = rs2[15:0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store 16-bits from lower bits of rs2 into memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m[rs1 + imm] = rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store rs2 into memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 + imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If (rs1 &lt; imm) rd = 1 else rd = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsigned comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 ^ imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 | imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &amp; imm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signed imm (Lower 5 bits)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &lt;&lt; imm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Unsigned imm Sign extend </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Lower 5 bits)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &gt;&gt; imm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Unsigned imm Unsigned shift </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Lower 5 bits)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Unsigned imm Signed shift </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">(Lower 5 bits)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rd, rs1, rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 + rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 – rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overflow is ignored</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &lt;&lt; rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower 5 bits of rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If (rs1 &lt; rs2) rd = 1 else rd = 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 ^ rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &gt;&gt; rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 | rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rd = rs1 &amp; rs2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pseudo Mnemonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MV</t>
   </si>
 </sst>
 </file>
@@ -464,7 +696,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -529,8 +761,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +803,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDAE3F3"/>
         <bgColor rgb="FFDEEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE994"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -637,7 +881,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -766,6 +1010,38 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -812,7 +1088,7 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFE2F0D9"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFE994"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
@@ -846,7 +1122,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1099,8 +1375,8 @@
   </sheetPr>
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M9" activeCellId="0" sqref="M9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1493,7 +1769,21 @@
       <c r="AF7" s="17"/>
       <c r="AG7" s="17"/>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="N9" s="17"/>
+      <c r="O9" s="17"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="17"/>
+      <c r="R9" s="17"/>
+      <c r="S9" s="17"/>
+      <c r="T9" s="17"/>
+      <c r="U9" s="17"/>
+    </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -5246,7 +5536,7 @@
       <selection pane="topLeft" activeCell="L40" activeCellId="0" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.11"/>
@@ -6692,6 +6982,681 @@
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:E69"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C43" activeCellId="0" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="36.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="47.4"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="34"/>
+    </row>
+    <row r="3" s="38" customFormat="true" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+      <c r="B3" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
+      <c r="B5" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
+      <c r="B6" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
+      <c r="B7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D7" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
+      <c r="B8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
+      <c r="B9" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="37" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="12" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0"/>
+      <c r="B12" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0"/>
+      <c r="B13" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0"/>
+      <c r="B14" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D14" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="37" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0"/>
+      <c r="B15" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="16" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0"/>
+      <c r="B16" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="18" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="37" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="21" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>176</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
+      <c r="B23" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D23" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="24" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D24" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="37" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="26" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="37" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="29" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>151</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="30" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="31" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="32" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="37" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="33" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="36" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D36" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E36" s="37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="37" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D37" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E37" s="37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D38" s="37" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="39" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="D39" s="37" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="40" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+    </row>
+    <row r="41" s="37" customFormat="true" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" s="32"/>
+    </row>
+    <row r="42" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="37" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+    </row>
+    <row r="45" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+    </row>
+    <row r="46" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0"/>
+    </row>
+    <row r="47" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0"/>
+    </row>
+    <row r="48" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0"/>
+    </row>
+    <row r="49" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+    </row>
+    <row r="50" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+    </row>
+    <row r="51" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+    </row>
+    <row r="52" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0"/>
+    </row>
+    <row r="53" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0"/>
+    </row>
+    <row r="54" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0"/>
+    </row>
+    <row r="55" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0"/>
+    </row>
+    <row r="56" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0"/>
+    </row>
+    <row r="57" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+    </row>
+    <row r="58" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+    </row>
+    <row r="59" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+    </row>
+    <row r="60" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0"/>
+    </row>
+    <row r="61" s="37" customFormat="true" ht="17.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0"/>
+    </row>
+    <row r="62" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0"/>
+      <c r="B62" s="0"/>
+      <c r="C62" s="0"/>
+      <c r="D62" s="0"/>
+    </row>
+    <row r="63" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="64" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="65" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="66" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="67" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="68" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="69" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B41:C41"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>